<commit_message>
updated measurements record type to include species & life stage
</commit_message>
<xml_diff>
--- a/JBER_new/JBER record types.xlsx
+++ b/JBER_new/JBER record types.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/school/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/school/Desktop/Salmon Project/data/JBER_new/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F8655A-06CE-ED4C-9D59-63B864A424D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AFC12E-4A34-534F-B626-E0B6FB65BDE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>17,71</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Last updated: 2/26</t>
+  </si>
+  <si>
+    <t>Life stage</t>
+  </si>
+  <si>
+    <t>Adult/smolt</t>
+  </si>
+  <si>
+    <t>str</t>
   </si>
 </sst>
 </file>
@@ -389,48 +398,48 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -441,7 +450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -452,15 +461,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -471,7 +480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -482,15 +491,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -500,11 +509,17 @@
       <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -513,6 +528,12 @@
       </c>
       <c r="C18" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>